<commit_message>
more tests and validation data, updated help
</commit_message>
<xml_diff>
--- a/s3tbx-fu-operator/src/ancillary/SNAP_CZCS.xlsx
+++ b/s3tbx-fu-operator/src/ancillary/SNAP_CZCS.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Projects\senbox\s3tbx\s3tbx-fu-operator\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="20115" windowHeight="7425" tabRatio="485"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="20115" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="My calculations " sheetId="1" r:id="rId1"/>
     <sheet name="spectra" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -112,15 +107,27 @@
     <t>Hans</t>
   </si>
   <si>
-    <t>SeaWiFS</t>
-  </si>
-  <si>
     <t>R670</t>
   </si>
   <si>
     <t xml:space="preserve">Pixel </t>
   </si>
   <si>
+    <t>HUESeaWiFS</t>
+  </si>
+  <si>
+    <t>HUESeaWiFS 100</t>
+  </si>
+  <si>
+    <t>Calculation POLYHueSeaWiFS</t>
+  </si>
+  <si>
+    <t>POLYHueSeaWiFS</t>
+  </si>
+  <si>
+    <t>HUESeaWiFSPcorr</t>
+  </si>
+  <si>
     <t>CZCS</t>
   </si>
   <si>
@@ -130,31 +137,13 @@
     <t>R550</t>
   </si>
   <si>
-    <t>COMPARE SNAP FU</t>
-  </si>
-  <si>
-    <t>HUE Pcorr</t>
-  </si>
-  <si>
-    <t>POLYHue</t>
-  </si>
-  <si>
-    <t>Calculation POLYHue</t>
-  </si>
-  <si>
-    <t>HUE</t>
-  </si>
-  <si>
-    <t>HUE 100</t>
-  </si>
-  <si>
-    <t>HUE Norm360</t>
+    <t xml:space="preserve">COMPARE SNAP V6 FU processor </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -173,12 +162,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,7 +197,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -212,15 +206,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -228,15 +228,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -278,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,26 +308,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -363,23 +343,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -556,18 +519,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -580,19 +541,19 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -609,24 +570,24 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="7">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="7">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -636,24 +597,24 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1.1E-4</v>
+      </c>
       <c r="E3" s="1">
-        <v>1.5686002000000001E-2</v>
+        <v>8.4999999999999995E-4</v>
       </c>
       <c r="F3" s="1">
-        <v>3.4360008000000001E-3</v>
+        <v>1.82E-3</v>
       </c>
       <c r="G3" s="1">
-        <v>1.9100008999999999E-3</v>
-      </c>
-      <c r="H3" s="9">
-        <v>2.8600087000000001E-4</v>
-      </c>
+        <v>1.1E-4</v>
+      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -681,19 +642,19 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
+      <c r="D5" s="8">
         <v>13.236774172196618</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="8">
         <v>5.1946800187878814</v>
       </c>
-      <c r="G5" s="2">
+      <c r="F5" s="8">
         <v>50.85635910558333</v>
       </c>
-      <c r="H5" s="2">
+      <c r="G5" s="8">
         <v>34.796598686583316</v>
       </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -720,28 +681,22 @@
       </c>
       <c r="D6" s="2">
         <f>D3*D5</f>
-        <v>0</v>
+        <v>1.4560451589416281E-3</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" ref="E6:I6" si="0">E3*E5</f>
-        <v>0.2076320661386245</v>
+        <f>E3*E5</f>
+        <v>4.4154780159696991E-3</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7848924700299175E-2</v>
+        <f>F3*F5</f>
+        <v>9.2558573572161656E-2</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>9.713569166238735E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>9.9518574974036857E-3</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <f>G3*G5</f>
+        <v>3.8276258555241648E-3</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -752,8 +707,8 @@
         <v>19</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" ref="P6:P12" si="1">SUM(D6:L6)</f>
-        <v>0.33256853999871472</v>
+        <f t="shared" ref="P6:P12" si="0">SUM(D6:L6)</f>
+        <v>0.10225772260259715</v>
       </c>
       <c r="T6" t="s">
         <v>0</v>
@@ -784,19 +739,19 @@
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="D8" s="8">
         <v>4.8252781922031129</v>
       </c>
-      <c r="F8" s="2">
+      <c r="E8" s="8">
         <v>25.217292711948041</v>
       </c>
-      <c r="G8" s="2">
+      <c r="F8" s="8">
         <v>56.9965040160833</v>
       </c>
-      <c r="H8" s="2">
+      <c r="G8" s="8">
         <v>19.570738452316665</v>
       </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -820,28 +775,22 @@
       </c>
       <c r="D9" s="2">
         <f>D8*D3</f>
-        <v>0</v>
+        <v>5.307806011423424E-4</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:I9" si="2">E8*E3</f>
-        <v>7.5689323373454423E-2</v>
+        <f t="shared" ref="E9:G9" si="1">E8*E3</f>
+        <v>2.1434698805155833E-2</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="2"/>
-        <v>8.6646637932087642E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.10373363730927161</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="2"/>
-        <v>0.10886337396757272</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="2"/>
-        <v>5.5972482239050195E-3</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>2.1527812297548331E-3</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -852,8 +801,8 @@
         <v>20</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" si="1"/>
-        <v>0.2767965834970198</v>
+        <f t="shared" si="0"/>
+        <v>0.12785189794532464</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -881,19 +830,19 @@
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
+      <c r="D11" s="8">
         <v>74.083470965457579</v>
       </c>
-      <c r="F11" s="2">
+      <c r="E11" s="8">
         <v>21.022899330161035</v>
       </c>
-      <c r="G11" s="2">
+      <c r="F11" s="8">
         <v>0.46162577510195829</v>
       </c>
-      <c r="H11" s="2">
+      <c r="G11" s="8">
         <v>2.1920674334041681E-2</v>
       </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -917,28 +866,22 @@
       </c>
       <c r="D12" s="2">
         <f>D11*D3</f>
-        <v>0</v>
+        <v>8.1491818062003341E-3</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" ref="E12:I12" si="3">E11*E3</f>
-        <v>1.1620734737311096</v>
+        <f t="shared" ref="E12:G12" si="2">E11*E3</f>
+        <v>1.7869464430636878E-2</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="3"/>
-        <v>7.2234698916752785E-2</v>
+        <f t="shared" si="2"/>
+        <v>8.401589106855641E-4</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="3"/>
-        <v>8.8170564590793791E-4</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="3"/>
-        <v>6.2693319305225912E-6</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>2.4112741767445852E-6</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -949,8 +892,8 @@
         <v>21</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" si="1"/>
-        <v>1.2351961476257007</v>
+        <f t="shared" si="0"/>
+        <v>2.6861216421699523E-2</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -974,11 +917,11 @@
       <c r="C14" s="2"/>
       <c r="D14">
         <f>P6/(P6+P9+P12)</f>
-        <v>0.18029682461918087</v>
+        <v>0.39793512683575799</v>
       </c>
       <c r="E14" s="2">
         <f>D14-0.333333</f>
-        <v>-0.15303617538081912</v>
+        <v>6.4602126835758E-2</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -997,11 +940,11 @@
       <c r="C15" s="2"/>
       <c r="D15">
         <f>P9/(P6+P9+P12)</f>
-        <v>0.15006093201161932</v>
+        <v>0.49753465978102057</v>
       </c>
       <c r="E15" s="2">
         <f>D15-0.333333</f>
-        <v>-0.18327206798838067</v>
+        <v>0.16420165978102058</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1015,7 +958,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -1023,11 +966,11 @@
       <c r="C16" s="2"/>
       <c r="D16">
         <f>180*ATAN2(D14-0.3333,D15-0.3333)/3.141527</f>
-        <v>-129.86432887923593</v>
+        <v>68.519139438449869</v>
       </c>
       <c r="E16" s="2">
         <f>ATAN2(E14,E15)</f>
-        <v>-2.2665302585591425</v>
+        <v>1.1959651299074465</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>0</v>
@@ -1041,14 +984,14 @@
       <c r="M16" s="2"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17">
-        <f>IF(D16&lt;0, D16+360,D16)</f>
-        <v>230.13567112076407</v>
+        <f>D16/100</f>
+        <v>0.68519139438449872</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1061,15 +1004,8 @@
       <c r="M17" s="2"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
-      <c r="D18">
-        <f>D17/100</f>
-        <v>2.3013567112076405</v>
-      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1081,185 +1017,176 @@
       <c r="M18" s="2"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
       <c r="C19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2">
+        <f>D17</f>
+        <v>0.68519139438449872</v>
+      </c>
+      <c r="D20" s="2">
+        <f>E20*C20</f>
+        <v>0.15102870522108663</v>
+      </c>
+      <c r="E20" s="2">
+        <f>F20*C20</f>
+        <v>0.22041827503796127</v>
+      </c>
+      <c r="F20" s="2">
+        <f>G20*C20</f>
+        <v>0.3216886213755808</v>
+      </c>
+      <c r="G20" s="2">
+        <f>H20*C20</f>
+        <v>0.46948724693857369</v>
+      </c>
+      <c r="H20" s="2">
+        <f>C20</f>
+        <v>0.68519139438449872</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="P20" s="3"/>
-      <c r="S20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="2">
-        <f>D18</f>
-        <v>2.3013567112076405</v>
-      </c>
-      <c r="D21" s="2">
-        <f>E21*C21</f>
-        <v>64.55348579641938</v>
-      </c>
-      <c r="E21" s="2">
-        <f>F21*C21</f>
-        <v>28.050186866748199</v>
-      </c>
-      <c r="F21" s="2">
-        <f>G21*C21</f>
-        <v>12.188543709953082</v>
-      </c>
-      <c r="G21" s="2">
-        <f>H21*C21</f>
-        <v>5.2962427122204474</v>
-      </c>
-      <c r="H21" s="2">
-        <f>C21</f>
-        <v>2.3013567112076405</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>-65.945183902456705</v>
+      </c>
+      <c r="E21" s="9">
+        <v>510.36869053864899</v>
+      </c>
+      <c r="F21" s="9">
+        <v>-1475.80076594513</v>
+      </c>
+      <c r="G21" s="9">
+        <v>1927.6141171593999</v>
+      </c>
+      <c r="H21" s="9">
+        <v>-1078.62361522692</v>
+      </c>
+      <c r="I21" s="9">
+        <v>202.245473021723</v>
       </c>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="8">
-        <v>-65.945183902456705</v>
-      </c>
-      <c r="E22" s="8">
-        <v>510.36869053864899</v>
-      </c>
-      <c r="F22" s="8">
-        <v>-1475.80076594513</v>
-      </c>
-      <c r="G22" s="8">
-        <v>1927.6141171593999</v>
-      </c>
-      <c r="H22" s="8">
-        <v>-1078.62361522692</v>
-      </c>
-      <c r="I22" s="8">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2">
+        <f>D20*D21</f>
+        <v>-9.9596157403544812</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" ref="E22:I22" si="3">E20*E21</f>
+        <v>112.49458640191207</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="3"/>
+        <v>-474.74831382191508</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="3"/>
+        <v>904.99024502509587</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="3"/>
+        <v>-739.06361893338237</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="3"/>
         <v>202.245473021723</v>
       </c>
       <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L22" s="2"/>
+      <c r="K22" s="2">
+        <f>SUM(D22:I22)</f>
+        <v>-4.0412440469209514</v>
+      </c>
+      <c r="L22" s="6"/>
       <c r="M22" s="2"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="2">
-        <f>D21*D22</f>
-        <v>-4256.991492389503</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" ref="E23:I23" si="4">E21*E22</f>
-        <v>14315.937140546688</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="4"/>
-        <v>-17987.862142904454</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="4"/>
-        <v>10209.112219978724</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="4"/>
-        <v>-2482.29769576952</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="4"/>
-        <v>202.245473021723</v>
-      </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2">
-        <f>SUM(D23:I23)</f>
-        <v>0.14350248365803964</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="P23" s="3">
-        <v>11.648</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2">
-        <f>K23</f>
-        <v>0.14350248365803964</v>
-      </c>
+      <c r="C24" s="2">
+        <f>K22</f>
+        <v>-4.0412440469209514</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1267,45 +1194,49 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="5"/>
+      <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="2">
-        <f>D16+C25</f>
-        <v>-129.72082639557789</v>
-      </c>
+      <c r="C26" s="2">
+        <f>D16+C24</f>
+        <v>64.477895391528918</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2">
+        <v>64.425179999999997</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="10">
+        <f>I26/C26</f>
+        <v>0.99918242691997283</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="2">
-        <v>99.757000000000005</v>
-      </c>
+      <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1313,8 +1244,16 @@
       <c r="N27" s="2"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1328,31 +1267,18 @@
       <c r="N28" s="2"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="P29" s="3"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1360,28 +1286,25 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="P33" s="3"/>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34">
-        <v>230.27994000000001</v>
-      </c>
-      <c r="G34" s="2">
-        <f>F34-360</f>
-        <v>-129.72005999999999</v>
-      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -1400,35 +1323,34 @@
       <c r="K35" s="2"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="P36" s="3"/>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="P39" s="3"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
@@ -1452,20 +1374,8 @@
       <c r="J41" s="2"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="P42" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1474,14 +1384,14 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D2" sqref="D2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -1498,21 +1408,17 @@
       <c r="G1" s="1">
         <v>4</v>
       </c>
-      <c r="H1" s="1">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1">
-        <v>6</v>
-      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1524,26 +1430,22 @@
         <v>1.1E-4</v>
       </c>
       <c r="E2" s="1">
-        <v>7.3999999999999999E-4</v>
+        <v>8.4999999999999995E-4</v>
       </c>
       <c r="F2" s="1">
-        <v>1.25E-3</v>
+        <v>1.82E-3</v>
       </c>
       <c r="G2" s="1">
-        <v>1.5900000000000001E-3</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1.7799999999999999E-3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3.4000000000000002E-4</v>
-      </c>
+        <v>1.1E-4</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1">
-        <v>138</v>
+        <v>1317</v>
       </c>
       <c r="L2" s="1">
-        <v>954</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>